<commit_message>
documento de excel de rechazo ya muestra pestaña para descargar excel
</commit_message>
<xml_diff>
--- a/My-App/public/volanteRechazo_dasdasdasdasdsadsa.xlsx
+++ b/My-App/public/volanteRechazo_dasdasdasdasdsadsa.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>DIRECCION GENERAL DE RECURSOS HUMANOS Y ORGANIZACIÓN</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>REVISÓ Y CAPTURÓ</t>
+  </si>
+  <si>
+    <t>Victor</t>
   </si>
   <si>
     <t>NOMBRE Y FIRMA</t>
@@ -1212,7 +1215,9 @@
       <c r="I31" s="19"/>
     </row>
     <row r="32" spans="1:15" customHeight="1" ht="12">
-      <c r="B32" s="17"/>
+      <c r="B32" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="C32" s="18"/>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -1225,7 +1230,7 @@
       <c r="B33" s="10"/>
       <c r="C33" s="11"/>
       <c r="D33" s="20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="20"/>
@@ -1235,7 +1240,7 @@
     </row>
     <row r="34" spans="1:15" customHeight="1" ht="15">
       <c r="B34" s="50" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C34" s="50"/>
       <c r="D34" s="50"/>
@@ -1267,7 +1272,7 @@
     </row>
     <row r="37" spans="1:15" customHeight="1" ht="18.75">
       <c r="B37" s="50" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C37" s="50"/>
       <c r="D37" s="50"/>
@@ -1299,7 +1304,7 @@
     </row>
     <row r="40" spans="1:15" customHeight="1" ht="15">
       <c r="B40" s="50" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C40" s="50"/>
       <c r="D40" s="50"/>

</xml_diff>